<commit_message>
Reprice test data excel update
</commit_message>
<xml_diff>
--- a/sales-e2e/resources/Reprice_Data/EstimatedCost_PVT_TestData.xlsx
+++ b/sales-e2e/resources/Reprice_Data/EstimatedCost_PVT_TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gegeorge/sales-e2e/sales-e2e/resources/Reprice_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0790CEB-2F33-CC41-96A3-7FA9262C7C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B427E74-3ABB-154A-9B52-799C89C49175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{E1B1B876-738B-914C-A22C-8BB86C52E263}"/>
+    <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" activeTab="3" xr2:uid="{E1B1B876-738B-914C-A22C-8BB86C52E263}"/>
   </bookViews>
   <sheets>
     <sheet name="RES-ELE" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="61">
   <si>
     <t>State</t>
   </si>
@@ -140,9 +140,6 @@
     <t>8 Popov Avenue, NEWINGTON NSW 2127</t>
   </si>
   <si>
-    <t>4 Rivage Court, HIGHLAND PARK QLD 4211</t>
-  </si>
-  <si>
     <t>EX</t>
   </si>
   <si>
@@ -152,12 +149,6 @@
     <t>QLD</t>
   </si>
   <si>
-    <t>24 Newton Street, NORTH EPPING NSW 2121</t>
-  </si>
-  <si>
-    <t>PKX</t>
-  </si>
-  <si>
     <t>7 Joseph Street, KINGSTON SE SA 5275</t>
   </si>
   <si>
@@ -198,13 +189,46 @@
   </si>
   <si>
     <t>UN</t>
+  </si>
+  <si>
+    <t>7 Gale Street, REDCLIFFE QLD 4020</t>
+  </si>
+  <si>
+    <t>70 Robertson Road, BASS HILL NSW 2197</t>
+  </si>
+  <si>
+    <t>PKX1</t>
+  </si>
+  <si>
+    <t>43 Trenchard Street, HEDDON GRETA NSW 2321</t>
+  </si>
+  <si>
+    <t>22 Ewan Street, MASCOT NSW 2020</t>
+  </si>
+  <si>
+    <t>PKXC</t>
+  </si>
+  <si>
+    <t>73 Cuthbert Street, HEATHMONT VIC 3135</t>
+  </si>
+  <si>
+    <t>8 Crockford Street, BENALLA VIC 3672</t>
+  </si>
+  <si>
+    <t>31 Tulloch Street, MILLGROVE VIC 3799</t>
+  </si>
+  <si>
+    <t>35 Aspen Street, MOONEE PONDS VIC 3039</t>
+  </si>
+  <si>
+    <t>31 Parkhurst Drive, KNOXFIELD VIC 3180</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -228,6 +252,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -285,11 +316,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -308,7 +340,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -596,7 +628,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -604,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1958B7-3DCC-1E4C-BEAA-B6FE28C9C060}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="124" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView zoomScale="124" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -636,7 +668,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -680,7 +712,7 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -715,7 +747,7 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
@@ -753,43 +785,43 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="I4" t="s">
         <v>7</v>
       </c>
       <c r="J4">
-        <v>2202</v>
+        <v>1453</v>
       </c>
       <c r="K4" t="s">
         <v>20</v>
       </c>
       <c r="L4">
-        <v>2202</v>
+        <v>1453</v>
       </c>
       <c r="M4" t="s">
         <v>8</v>
       </c>
       <c r="N4">
-        <v>2202</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -800,16 +832,16 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
         <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="G5" t="s">
         <v>19</v>
@@ -818,39 +850,33 @@
         <v>7</v>
       </c>
       <c r="J5">
-        <v>1469</v>
+        <v>1439</v>
       </c>
       <c r="K5" t="s">
         <v>20</v>
       </c>
       <c r="L5">
-        <v>1546</v>
-      </c>
-      <c r="M5" t="s">
-        <v>8</v>
-      </c>
-      <c r="N5">
-        <v>1546</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
         <v>19</v>
@@ -872,6 +898,47 @@
       </c>
       <c r="N6">
         <v>1743</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <v>1225</v>
+      </c>
+      <c r="K7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7">
+        <v>1290</v>
+      </c>
+      <c r="M7" t="s">
+        <v>8</v>
+      </c>
+      <c r="N7">
+        <v>1290</v>
       </c>
     </row>
   </sheetData>
@@ -882,10 +949,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A06D330F-ACA0-B64A-85A5-282398920C4E}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView zoomScale="173" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -905,7 +972,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -946,10 +1013,10 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -958,19 +1025,19 @@
         <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G2" t="s">
         <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J2">
         <v>2739</v>
       </c>
       <c r="K2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L2">
         <v>2682</v>
@@ -978,34 +1045,34 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
         <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G3" t="s">
         <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J3">
         <v>4043</v>
       </c>
       <c r="K3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L3">
         <v>3959</v>
@@ -1016,34 +1083,69 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
         <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G4" t="s">
         <v>22</v>
       </c>
       <c r="I4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J4">
         <v>776</v>
       </c>
       <c r="K4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L4">
         <v>760</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5">
+        <v>2974</v>
+      </c>
+      <c r="K5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5">
+        <v>2913</v>
       </c>
     </row>
   </sheetData>
@@ -1053,10 +1155,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5F80D7-3027-A243-AD13-F8BA8FB6B42C}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1085,7 +1187,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1129,25 +1231,25 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="I2" t="s">
         <v>7</v>
       </c>
       <c r="J2">
-        <v>1588</v>
+        <v>3243</v>
       </c>
       <c r="K2" t="s">
         <v>20</v>
       </c>
       <c r="L2">
-        <v>1804</v>
+        <v>3685</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -1158,7 +1260,7 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
         <v>24</v>
@@ -1187,7 +1289,7 @@
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F4" t="s">
         <v>32</v>
@@ -1210,16 +1312,16 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G5" t="s">
         <v>19</v>
@@ -1235,6 +1337,64 @@
       </c>
       <c r="L5">
         <v>1252</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6">
+        <v>3334</v>
+      </c>
+      <c r="K6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6">
+        <v>3788</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <v>3377</v>
+      </c>
+      <c r="K7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7">
+        <v>3838</v>
       </c>
     </row>
   </sheetData>
@@ -1244,10 +1404,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB041EC-154A-F54F-B467-E591D8104C80}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1276,7 +1436,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1317,19 +1477,19 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
         <v>42</v>
-      </c>
-      <c r="C2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" t="s">
-        <v>45</v>
       </c>
       <c r="G2" t="s">
         <v>19</v>
       </c>
       <c r="K2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L2">
         <v>4480</v>
@@ -1340,22 +1500,45 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L3">
-        <v>1039</v>
+        <v>3141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4">
+        <v>10888</v>
       </c>
     </row>
   </sheetData>

</xml_diff>